<commit_message>
Updated policies and graphs
</commit_message>
<xml_diff>
--- a/Assembled Data/grocerypharma_mobility.xlsx
+++ b/Assembled Data/grocerypharma_mobility.xlsx
@@ -533,13 +533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:HF53"/>
+  <dimension ref="A1:HQ53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:214">
+    <row r="1" spans="1:225">
       <c r="B1" s="1">
         <v>43891</v>
       </c>
@@ -1179,8 +1179,41 @@
       <c r="HF1" s="1">
         <v>44103</v>
       </c>
+      <c r="HG1" s="1">
+        <v>44104</v>
+      </c>
+      <c r="HH1" s="1">
+        <v>44105</v>
+      </c>
+      <c r="HI1" s="1">
+        <v>44106</v>
+      </c>
+      <c r="HJ1" s="1">
+        <v>44107</v>
+      </c>
+      <c r="HK1" s="1">
+        <v>44108</v>
+      </c>
+      <c r="HL1" s="1">
+        <v>44109</v>
+      </c>
+      <c r="HM1" s="1">
+        <v>44110</v>
+      </c>
+      <c r="HN1" s="1">
+        <v>44111</v>
+      </c>
+      <c r="HO1" s="1">
+        <v>44112</v>
+      </c>
+      <c r="HP1" s="1">
+        <v>44113</v>
+      </c>
+      <c r="HQ1" s="1">
+        <v>44114</v>
+      </c>
     </row>
-    <row r="2" spans="1:214">
+    <row r="2" spans="1:225">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1587,7 +1620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:214">
+    <row r="3" spans="1:225">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1994,7 +2027,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="4" spans="1:214">
+    <row r="4" spans="1:225">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2401,7 +2434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:214">
+    <row r="5" spans="1:225">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2808,7 +2841,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="6" spans="1:214">
+    <row r="6" spans="1:225">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -3215,7 +3248,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:214">
+    <row r="7" spans="1:225">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -3622,7 +3655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:214">
+    <row r="8" spans="1:225">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -4029,7 +4062,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="9" spans="1:214">
+    <row r="9" spans="1:225">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -4436,7 +4469,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="10" spans="1:214">
+    <row r="10" spans="1:225">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -4843,7 +4876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:214">
+    <row r="11" spans="1:225">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -5250,7 +5283,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="12" spans="1:214">
+    <row r="12" spans="1:225">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -5657,7 +5690,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="13" spans="1:214">
+    <row r="13" spans="1:225">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -6064,7 +6097,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="14" spans="1:214">
+    <row r="14" spans="1:225">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -6471,7 +6504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:214">
+    <row r="15" spans="1:225">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -6878,7 +6911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:214">
+    <row r="16" spans="1:225">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>